<commit_message>
Fix field validation and UI guide in Excel upload
- Fix critical variable declaration order issue in server code
- Move standardFieldMappings and requiredStandardFields to top of file
- Add comprehensive logging for debugging field validation
- Enhance error messages with clear field name corrections
- Update all test Excel files to match standard template format
- Add field guide alert in UI with template download button
- Implement strict field name validation with detailed feedback

This ensures:
1. Field guide message always appears in upload UI
2. Incorrect field names are properly detected and reported
3. Users receive clear guidance on correct field names
4. All test files now use standard template format

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/PO_test/generated_test_files/TestPO_01_티에스이앤씨_1_6items.xlsx
+++ b/PO_test/generated_test_files/TestPO_01_티에스이앤씨_1_6items.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Input" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="갑지" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="을지" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Input" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="갑지" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="을지" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,87 +436,82 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>발주일자</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>납기일자</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>거래처명</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>현장명</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>발주일</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>납기일</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>발주번호</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>품목</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>거래처 이메일</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>납품처명</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>납품처 이메일</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>프로젝트명</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>대분류</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>중분류</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>소분류</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>품목명</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
         <is>
           <t>규격</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>수량</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>단위</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>단가</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>공급가액</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>부가세</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>합계</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>대분류</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>중분류</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>소분류</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>총금액</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
         <is>
           <t>비고</t>
         </is>
@@ -525,440 +520,429 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>티에스이앤씨</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>티에스이앤씨@example.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>힐스테이트 도곡동1차</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-08-22</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-08-29</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>PO-20250819-티에스-920</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>delivery@example.com</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>힐스테이트 도곡동1차</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>6. 안전관리비</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1) 안전장비</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>안전 1차 - 안전벨트</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>KS규격-1</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="M2" t="n">
         <v>5</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>37000</v>
       </c>
-      <c r="K2" t="n">
-        <v>185000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>18500</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>203500</v>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>6. 안전관리비</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1) 안전장비</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>티에스이앤씨</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>티에스이앤씨@example.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>힐스테이트 도곡동1차</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-09-17</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-10-03</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>PO-20250819-티에스-114</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>delivery@example.com</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>힐스테이트 도곡동1차</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>6. 안전관리비</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1) 안전장비</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>화재감시자 안전모</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>KS규격-2</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="M3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>6000</v>
       </c>
-      <c r="K3" t="n">
-        <v>6000</v>
-      </c>
-      <c r="L3" t="n">
-        <v>600</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>6600</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>6. 안전관리비</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>1) 안전장비</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>티에스이앤씨</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>티에스이앤씨@example.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>힐스테이트 도곡동1차</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-08-29</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-10-01</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>PO-20250819-티에스-146</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>delivery@example.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>힐스테이트 도곡동1차</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2. 부자재비</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2) 창호</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
           <t>3차 - 스크류 (둥근머리 8*25)</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>KS규격-3</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="M4" t="n">
         <v>500</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
+      <c r="N4" t="n">
         <v>19</v>
       </c>
-      <c r="K4" t="n">
-        <v>9500</v>
-      </c>
-      <c r="L4" t="n">
-        <v>950</v>
-      </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>10450</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>2. 부자재비</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>2) 창호</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>티에스이앤씨</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>티에스이앤씨@example.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>힐스테이트 도곡동1차</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-08-29</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-09-22</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>PO-20250819-티에스-257</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>delivery@example.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>힐스테이트 도곡동1차</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2. 부자재비</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2) 창호</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>화기감시자 조끼(적색)</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>KS규격-4</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="M5" t="n">
         <v>2</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
+      <c r="N5" t="n">
         <v>8000</v>
       </c>
-      <c r="K5" t="n">
-        <v>16000</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1600</v>
-      </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>17600</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>2. 부자재비</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2) 창호</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>티에스이앤씨</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>티에스이앤씨@example.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>힐스테이트 도곡동1차</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-10-16</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>PO-20250819-티에스-344</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>delivery@example.com</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>힐스테이트 도곡동1차</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2. 부자재비</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2) 창호</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
           <t>칼블럭 8*70</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>KS규격-5</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="M6" t="n">
         <v>1000</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
+      <c r="N6" t="n">
         <v>119</v>
       </c>
-      <c r="K6" t="n">
-        <v>119000</v>
-      </c>
-      <c r="L6" t="n">
-        <v>11900</v>
-      </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>130900</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>2. 부자재비</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>2) 창호</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>티에스이앤씨</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>티에스이앤씨@example.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>힐스테이트 도곡동1차</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-08-27</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-10-08</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>PO-20250819-티에스-845</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>delivery@example.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>힐스테이트 도곡동1차</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2. 부자재비</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2) 창호</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>2차 - 타격공구</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>KS규격-6</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="M7" t="n">
         <v>2</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>EA</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
+      <c r="N7" t="n">
         <v>17500</v>
       </c>
-      <c r="K7" t="n">
-        <v>35000</v>
-      </c>
-      <c r="L7" t="n">
-        <v>3500</v>
-      </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>38500</v>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>2. 부자재비</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2) 창호</t>
-        </is>
-      </c>
       <c r="P7" t="inlineStr">
-        <is>
-          <t>기타</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
         <is>
           <t>2차</t>
         </is>
@@ -1061,7 +1045,6 @@
       <c r="H2" t="n">
         <v>203500</v>
       </c>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1094,7 +1077,6 @@
       <c r="H3" t="n">
         <v>6600</v>
       </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1127,7 +1109,6 @@
       <c r="H4" t="n">
         <v>10450</v>
       </c>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1160,7 +1141,6 @@
       <c r="H5" t="n">
         <v>17600</v>
       </c>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1193,7 +1173,6 @@
       <c r="H6" t="n">
         <v>130900</v>
       </c>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1329,7 +1308,6 @@
       <c r="H2" t="n">
         <v>203500</v>
       </c>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1362,7 +1340,6 @@
       <c r="H3" t="n">
         <v>6600</v>
       </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1395,7 +1372,6 @@
       <c r="H4" t="n">
         <v>10450</v>
       </c>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1428,7 +1404,6 @@
       <c r="H5" t="n">
         <v>17600</v>
       </c>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1461,7 +1436,6 @@
       <c r="H6" t="n">
         <v>130900</v>
       </c>
-      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">

</xml_diff>